<commit_message>
Rings colors and logic
Modified rings color
Added inring-intraring-bias-pct
</commit_message>
<xml_diff>
--- a/excel/marslink.xlsx
+++ b/excel/marslink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Documents\git\marslink\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2A975C-7FA3-440C-A3F2-AEFBA4CEAE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1607DAE4-603D-472F-9941-392E0727098E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{9A5CB930-BBE5-432A-9FE8-5E7087FDEBF4}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>radius</t>
   </si>
@@ -230,6 +230,78 @@
   </si>
   <si>
     <t>satcount chosen</t>
+  </si>
+  <si>
+    <t>Case 1: aligned</t>
+  </si>
+  <si>
+    <t>Case 2: opposed</t>
+  </si>
+  <si>
+    <t>all interring</t>
+  </si>
+  <si>
+    <t>all inring</t>
+  </si>
+  <si>
+    <t>In-ring mbps</t>
+  </si>
+  <si>
+    <t>sats per ring</t>
+  </si>
+  <si>
+    <t>satisfies A</t>
+  </si>
+  <si>
+    <t>in-ring mbps</t>
+  </si>
+  <si>
+    <t>A (in-ring)</t>
+  </si>
+  <si>
+    <t>total inter-ring mbps</t>
+  </si>
+  <si>
+    <t>unit inter-ring mbps</t>
+  </si>
+  <si>
+    <t>inter-ring distance</t>
+  </si>
+  <si>
+    <t>mbps</t>
+  </si>
+  <si>
+    <t>System / B (inter-ring)</t>
+  </si>
+  <si>
+    <t>sats per ring to satisfy A</t>
+  </si>
+  <si>
+    <t>system mbps</t>
+  </si>
+  <si>
+    <t>input system mbps</t>
+  </si>
+  <si>
+    <t>total sats</t>
+  </si>
+  <si>
+    <t>setup cost k$</t>
+  </si>
+  <si>
+    <t>variable cost (wright's law) k$</t>
+  </si>
+  <si>
+    <t>total cost m$</t>
+  </si>
+  <si>
+    <t>improvement 100x</t>
+  </si>
+  <si>
+    <t>Earth ring full</t>
+  </si>
+  <si>
+    <t>Mars ring?</t>
   </si>
 </sst>
 </file>
@@ -237,9 +309,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="178" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -290,10 +362,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -302,10 +374,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -322,6 +393,1326 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Marslink performance vs. cost</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-150"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>system mbps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$16:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$16:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34.127824278652923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131.15735152727268</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>373.34465486043132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>865.36366511936649</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1737.7704886049646</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3149.5229108835697</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5291.8741753959539</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8376.5484940050701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12649.054334151733</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E482-49B3-9CFB-8F0862CD2CB4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="538215871"/>
+        <c:axId val="541547231"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total sats</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$16:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$16:$Q$24</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2445</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4836</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13470</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20216</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28896</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39762</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-E482-49B3-9CFB-8F0862CD2CB4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total cost m$</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$16:$L$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$16:$S$24</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4809.0320220750054</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10995.938242022641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19876.820256049508</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31533.405722498992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45939.264351311256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63103.794920390901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83085.033497601355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105840.8191692273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>131402.83596207801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-E482-49B3-9CFB-8F0862CD2CB4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="450620543"/>
+        <c:axId val="450614783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="538215871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="541547231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="541547231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="538215871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="450614783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450620543"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="450620543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="450614783"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-150"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-150"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>588168</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>626268</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575B040C-7051-F0BF-6CE6-AFEA665FC4CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -641,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B6E028-3455-4EC3-BC04-5235B4A58697}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -654,9 +2045,11 @@
     <col min="4" max="5" width="12.9296875" customWidth="1"/>
     <col min="6" max="7" width="9.06640625" style="8"/>
     <col min="8" max="8" width="11.73046875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -667,7 +2060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
@@ -675,7 +2068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -689,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -706,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -729,7 +2122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -752,7 +2145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="K8" t="s">
         <v>5</v>
       </c>
@@ -760,7 +2153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -771,13 +2164,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <f>B40</f>
-        <v>1.0515886039697149</v>
+        <v>1.0970990292388583</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -789,13 +2182,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <f>C40</f>
-        <v>1809</v>
+        <v>280</v>
       </c>
       <c r="K11" t="s">
         <v>8</v>
@@ -804,13 +2197,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <f>2*B10*SIN(PI()/B11)</f>
-        <v>3.6524724955470786E-3</v>
+        <v>2.4618328114392046E-2</v>
       </c>
       <c r="C12" t="str">
         <f>$C$10</f>
@@ -823,25 +2216,69 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
         <f>2*PI()*B10/B11</f>
-        <v>3.6524743314870121E-3</v>
+        <v>2.4618844646552077E-2</v>
       </c>
       <c r="C13" t="str">
         <f>$C$10</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="R13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S13">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="L14" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="4">
+        <v>23.2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" t="s">
+        <v>63</v>
+      </c>
+      <c r="P15" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>73</v>
+      </c>
+      <c r="R15" t="s">
+        <v>75</v>
+      </c>
+      <c r="S15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -853,8 +2290,48 @@
         <f>$D$4</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <f>I15/2</f>
+        <v>11.6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>34</v>
+      </c>
+      <c r="N16">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M16/2/1024)))/km_per_AU)/2/($B$16+$B$18/L16/2)),0)</f>
+        <v>298</v>
+      </c>
+      <c r="O16">
+        <f>(($A$25*(L16+1)/$D$18)^2)*$B$25*$B$27*N16/2*1024</f>
+        <v>17.063912139326462</v>
+      </c>
+      <c r="P16" s="8">
+        <f>O16*2</f>
+        <v>34.127824278652923</v>
+      </c>
+      <c r="Q16" s="8">
+        <f>N16*L16</f>
+        <v>298</v>
+      </c>
+      <c r="R16" s="8">
+        <f>100000*Q16^-0.322</f>
+        <v>15969.906114345658</v>
+      </c>
+      <c r="S16" s="8">
+        <f>($S$13+R16*Q16)/1000</f>
+        <v>4809.0320220750054</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -866,8 +2343,39 @@
         <f>$D$4</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="L17">
+        <f>L16+1</f>
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>131</v>
+      </c>
+      <c r="N17">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M17/2/1024)))/km_per_AU)/2/($B$16+$B$18/L17/2)),0)</f>
+        <v>509</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17:O18" si="0">(($A$25*(L17+1)/$D$18)^2)*$B$25*$B$27*N17/2*1024</f>
+        <v>65.57867576363634</v>
+      </c>
+      <c r="P17" s="8">
+        <f t="shared" ref="P17:P27" si="1">O17*2</f>
+        <v>131.15735152727268</v>
+      </c>
+      <c r="Q17" s="8">
+        <f t="shared" ref="Q17:Q24" si="2">N17*L17</f>
+        <v>1018</v>
+      </c>
+      <c r="R17" s="8">
+        <f t="shared" ref="R17:R24" si="3">100000*Q17^-0.322</f>
+        <v>10752.395129688253</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" ref="S17:S24" si="4">($S$13+R17*Q17)/1000</f>
+        <v>10995.938242022641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -879,70 +2387,354 @@
         <f>$D$4</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" s="8">
+        <f>B18*km_per_AU</f>
+        <v>102123940.72372979</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="8">
+        <f>A25*SQRT($B$25*$B$27/(I16/1024))</f>
+        <v>5073582.6966070374</v>
+      </c>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L20" si="5">L17+1</f>
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>373</v>
+      </c>
+      <c r="N18">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M18/2/1024)))/km_per_AU)/2/($B$16+$B$18/L18/2)),0)</f>
+        <v>815</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>186.67232743021566</v>
+      </c>
+      <c r="P18" s="8">
+        <f t="shared" si="1"/>
+        <v>373.34465486043132</v>
+      </c>
+      <c r="Q18" s="8">
+        <f t="shared" si="2"/>
+        <v>2445</v>
+      </c>
+      <c r="R18" s="8">
+        <f t="shared" si="3"/>
+        <v>8109.1289390795546</v>
+      </c>
+      <c r="S18" s="8">
+        <f t="shared" si="4"/>
+        <v>19876.820256049508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19">
+        <f>I18/km_per_AU</f>
+        <v>3.3914805557503418E-2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>865</v>
+      </c>
+      <c r="N19">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M19/2/1024)))/km_per_AU)/2/($B$16+$B$18/L19/2)),0)</f>
+        <v>1209</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O20" si="6">(($A$25*(L19+1)/$D$18)^2)*$B$25*$B$27*N19/2*1024</f>
+        <v>432.68183255968324</v>
+      </c>
+      <c r="P19" s="8">
+        <f t="shared" si="1"/>
+        <v>865.36366511936649</v>
+      </c>
+      <c r="Q19" s="8">
+        <f t="shared" si="2"/>
+        <v>4836</v>
+      </c>
+      <c r="R19" s="8">
+        <f t="shared" si="3"/>
+        <v>6510.216237075887</v>
+      </c>
+      <c r="S19" s="8">
+        <f t="shared" si="4"/>
+        <v>31533.405722498992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="3">
         <f>B18/B19/2</f>
-        <v>6.8265637903715023E-2</v>
+        <v>0.11377606317285838</v>
       </c>
       <c r="C20" t="str">
         <f>$D$4</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="3">
+        <f>B16+B18/L16/2</f>
+        <v>1.324651155584575</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>1737</v>
+      </c>
+      <c r="N20">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M20/2/1024)))/km_per_AU)/2/($B$16+$B$18/L20/2)),0)</f>
+        <v>1686</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>868.88524430248231</v>
+      </c>
+      <c r="P20" s="8">
+        <f t="shared" si="1"/>
+        <v>1737.7704886049646</v>
+      </c>
+      <c r="Q20" s="8">
+        <f t="shared" si="2"/>
+        <v>8430</v>
+      </c>
+      <c r="R20" s="8">
+        <f t="shared" si="3"/>
+        <v>5443.5663524687143</v>
+      </c>
+      <c r="S20" s="8">
+        <f t="shared" si="4"/>
+        <v>45939.264351311256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="3">
         <f>B20*2</f>
-        <v>0.13653127580743005</v>
+        <v>0.22755212634571675</v>
       </c>
       <c r="C21" t="str">
         <f>$D$4</f>
         <v>AU</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21">
+        <f>ROUNDUP(PI()/ASIN(I19/2/I20),0)</f>
+        <v>246</v>
+      </c>
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21:L25" si="7">L20+1</f>
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>3148</v>
+      </c>
+      <c r="N21">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M21/2/1024)))/km_per_AU)/2/($B$16+$B$18/L21/2)),0)</f>
+        <v>2245</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ref="O21:O25" si="8">(($A$25*(L21+1)/$D$18)^2)*$B$25*$B$27*N21/2*1024</f>
+        <v>1574.7614554417848</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="shared" si="1"/>
+        <v>3149.5229108835697</v>
+      </c>
+      <c r="Q21" s="8">
+        <f t="shared" si="2"/>
+        <v>13470</v>
+      </c>
+      <c r="R21" s="8">
+        <f t="shared" si="3"/>
+        <v>4681.053817400958</v>
+      </c>
+      <c r="S21" s="8">
+        <f t="shared" si="4"/>
+        <v>63103.794920390901</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="3">
         <f>B16+B20</f>
-        <v>1.0515886039697149</v>
+        <v>1.0970990292388583</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22">
+        <f>B25*B27/(I18/A25)^2*1024</f>
+        <v>11.600000000000005</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="M22">
+        <v>5290</v>
+      </c>
+      <c r="N22">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M22/2/1024)))/km_per_AU)/2/($B$16+$B$18/L22/2)),0)</f>
+        <v>2888</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="8"/>
+        <v>2645.9370876979769</v>
+      </c>
+      <c r="P22" s="8">
+        <f t="shared" si="1"/>
+        <v>5291.8741753959539</v>
+      </c>
+      <c r="Q22" s="8">
+        <f t="shared" si="2"/>
+        <v>20216</v>
+      </c>
+      <c r="R22" s="8">
+        <f t="shared" si="3"/>
+        <v>4107.3918429759278</v>
+      </c>
+      <c r="S22" s="8">
+        <f t="shared" si="4"/>
+        <v>83085.033497601355</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>8376</v>
+      </c>
+      <c r="N23">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M23/2/1024)))/km_per_AU)/2/($B$16+$B$18/L23/2)),0)</f>
+        <v>3612</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="8"/>
+        <v>4188.274247002535</v>
+      </c>
+      <c r="P23" s="8">
+        <f t="shared" si="1"/>
+        <v>8376.5484940050701</v>
+      </c>
+      <c r="Q23" s="8">
+        <f t="shared" si="2"/>
+        <v>28896</v>
+      </c>
+      <c r="R23" s="8">
+        <f t="shared" si="3"/>
+        <v>3661.0887032539904</v>
+      </c>
+      <c r="S23" s="8">
+        <f t="shared" si="4"/>
+        <v>105840.8191692273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24">
+        <f>SQRT(2*I16/1024/B25/B27/I21)*D18/A25-1</f>
+        <v>0.81493161400017966</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="M24">
+        <v>12649</v>
+      </c>
+      <c r="N24">
+        <f>ROUNDUP(PI()/ASIN((($A$25*SQRT($B$25*$B$27/(M24/2/1024)))/km_per_AU)/2/($B$16+$B$18/L24/2)),0)</f>
+        <v>4418</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="8"/>
+        <v>6324.5271670758666</v>
+      </c>
+      <c r="P24" s="8">
+        <f t="shared" si="1"/>
+        <v>12649.054334151733</v>
+      </c>
+      <c r="Q24" s="8">
+        <f t="shared" si="2"/>
+        <v>39762</v>
+      </c>
+      <c r="R24" s="8">
+        <f t="shared" si="3"/>
+        <v>3303.4765847311005</v>
+      </c>
+      <c r="S24" s="8">
+        <f t="shared" si="4"/>
+        <v>131402.83596207801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>5400</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <f>ROUNDUP(I24,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26">
         <f>A25*2</f>
         <v>10800</v>
@@ -951,105 +2743,159 @@
         <f>B25/(A26/A25)^2</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="L26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27">
+        <f>((A25*(I25+1)/D18)^2)*B25*B27*I21/2*1024</f>
+        <v>14.086316732464125</v>
+      </c>
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="H28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="8">
+        <f>D18/(I25+1)</f>
+        <v>51061970.361864895</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29">
+        <f>$B$25*$B$27/(I28/$A$25)^2*1024</f>
+        <v>0.11452290026393597</v>
+      </c>
+      <c r="J29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="4">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="H30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30">
+        <f>I29*I21</f>
+        <v>28.172633464928246</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="8">
         <f>A25*SQRT($B$25*$B$27/(B30/1024))</f>
-        <v>546441.57967709599</v>
+        <v>3684108.3786249482</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32">
         <f>B31/km_per_AU</f>
-        <v>3.6527363465815427E-3</v>
+        <v>2.4626743424797613E-2</v>
       </c>
       <c r="C32" t="str">
         <f>$D$4</f>
         <v>AU</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>18</v>
       </c>
       <c r="B35" s="8">
         <f>B21*km_per_AU</f>
-        <v>20424788.144745957</v>
+        <v>34041313.574576594</v>
       </c>
       <c r="C35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="2">
         <f>$B$25*$B$27/(B35/$A$25)^2*1024</f>
-        <v>7.1576812664959993E-2</v>
+        <v>0.25767652559385601</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C38" s="13">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C38" s="12">
         <f>SUM(_xlfn.ANCHORARRAY(C40))</f>
-        <v>11395</v>
+        <v>1015</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="12">
         <f>SUM(E40:E44)</f>
-        <v>10690</v>
+        <v>840</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>28</v>
       </c>
@@ -1074,290 +2920,263 @@
       <c r="H39" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="J39" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" cm="1">
-        <f t="array" ref="A40:A44">_xlfn.SEQUENCE(B19)</f>
+        <f t="array" ref="A40:A42">_xlfn.SEQUENCE(B19)</f>
         <v>1</v>
       </c>
       <c r="B40" cm="1">
-        <f t="array" ref="B40:B44">$B$22+(_xlfn.SEQUENCE(B19)-1)*$B$21</f>
-        <v>1.0515886039697149</v>
+        <f t="array" ref="B40:B42">$B$22+(_xlfn.SEQUENCE(B19)-1)*$B$21</f>
+        <v>1.0970990292388583</v>
       </c>
       <c r="C40" s="7" cm="1">
-        <f t="array" ref="C40:C44">ROUNDUP(PI()/ASIN($B$32/(2*(INDEX(_xlfn.ANCHORARRAY(B40),_xlfn.SEQUENCE(B19))))),0)</f>
-        <v>1809</v>
+        <f t="array" ref="C40:C42">ROUNDUP(PI()/ASIN($B$32/(2*(INDEX(_xlfn.ANCHORARRAY(B40),_xlfn.SEQUENCE(B19))))),0)</f>
+        <v>280</v>
       </c>
       <c r="D40" s="7" cm="1">
-        <f t="array" ref="D40:D44">IF(_xlfn.SEQUENCE(ring_count),C40)</f>
-        <v>1809</v>
+        <f t="array" ref="D40:D42">IF(_xlfn.SEQUENCE(ring_count),C40)</f>
+        <v>280</v>
       </c>
       <c r="E40" s="7">
-        <f>AVERAGE(C40:D40)</f>
-        <v>1809</v>
+        <f>D40</f>
+        <v>280</v>
       </c>
       <c r="F40" s="8" cm="1">
-        <f t="array" ref="F40:F44">2*INDEX(_xlfn.ANCHORARRAY(B40),_xlfn.SEQUENCE(B19))*SIN(PI()/INDEX(E40:E44,_xlfn.SEQUENCE(B19)))*km_per_AU</f>
-        <v>546402.10812415811</v>
+        <f t="array" ref="F40:F42">2*INDEX(_xlfn.ANCHORARRAY(B40),_xlfn.SEQUENCE(B19))*SIN(PI()/INDEX(E40:E44,_xlfn.SEQUENCE(B19)))*km_per_AU</f>
+        <v>3682849.4661069959</v>
       </c>
       <c r="G40" s="8" cm="1">
-        <f t="array" ref="G40:G44">$B$25*$B$27/((INDEX(_xlfn.ANCHORARRAY(F40),_xlfn.SEQUENCE(B19)))/$A$25)^2*1024</f>
-        <v>100.01444832589189</v>
+        <f t="array" ref="G40:G42">$B$25*$B$27/((INDEX(_xlfn.ANCHORARRAY(F40),_xlfn.SEQUENCE(B19)))/$A$25)^2*1024</f>
+        <v>22.015043139471196</v>
       </c>
       <c r="H40" s="8">
         <f>IF(E41,MIN(E40,E41)*$B$36,"")</f>
-        <v>129.48245411091264</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+        <v>72.149427166279679</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41">
-        <v>1.1881198797771448</v>
+        <v>1.324651155584575</v>
       </c>
       <c r="C41" s="7">
-        <v>2044</v>
+        <v>338</v>
       </c>
       <c r="D41">
-        <v>1809</v>
+        <v>280</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" ref="E41:E44" si="0">AVERAGE(C41:D41)</f>
-        <v>1926.5</v>
+        <f t="shared" ref="E41:E44" si="9">D41</f>
+        <v>280</v>
       </c>
       <c r="F41" s="8">
-        <v>579690.70555411407</v>
+        <v>4446718.7292174073</v>
       </c>
       <c r="G41" s="8">
-        <v>88.857645612576363</v>
+        <v>15.101085170135374</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" ref="H41:H57" si="1">IF(E42,MIN(E41,E42)*$B$36,"")</f>
-        <v>137.89272959904542</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+        <f t="shared" ref="H41:H57" si="10">IF(E42,MIN(E41,E42)*$B$36,"")</f>
+        <v>72.149427166279679</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42">
-        <v>1.324651155584575</v>
+        <v>1.5522032819302918</v>
       </c>
       <c r="C42" s="7">
-        <v>2279</v>
+        <v>397</v>
       </c>
       <c r="D42">
-        <v>1809</v>
+        <v>280</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="0"/>
-        <v>2044</v>
+        <f t="shared" si="9"/>
+        <v>280</v>
       </c>
       <c r="F42" s="8">
-        <v>609152.09284111543</v>
+        <v>5210587.9923278196</v>
       </c>
       <c r="G42" s="8">
-        <v>80.470369408521918</v>
-      </c>
-      <c r="H42" s="8">
-        <f t="shared" si="1"/>
-        <v>146.30300508717824</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43">
-        <v>1.461182431392005</v>
-      </c>
-      <c r="C43" s="7">
-        <v>2514</v>
-      </c>
-      <c r="D43">
-        <v>1809</v>
-      </c>
+        <v>10.998007402175698</v>
+      </c>
+      <c r="H42" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C43" s="7"/>
       <c r="E43" s="7">
-        <f t="shared" si="0"/>
-        <v>2161.5</v>
-      </c>
-      <c r="F43" s="8">
-        <v>635410.41554767382</v>
-      </c>
-      <c r="G43" s="8">
-        <v>73.956920190587738</v>
-      </c>
-      <c r="H43" s="8">
-        <f t="shared" si="1"/>
-        <v>154.71328057531102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="B44">
-        <v>1.5977137071994352</v>
-      </c>
-      <c r="C44" s="7">
-        <v>2749</v>
-      </c>
-      <c r="D44">
-        <v>1809</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="8" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C44" s="7"/>
       <c r="E44" s="7">
-        <f>C44</f>
-        <v>2749</v>
-      </c>
-      <c r="F44" s="8">
-        <v>546297.74414166622</v>
-      </c>
-      <c r="G44" s="8">
-        <v>100.05266522598968</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="H44" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F45" s="8" t="str">
-        <f t="shared" ref="F41:F58" si="2">IF(C46,MIN(C45,C46)*$B$36,"")</f>
+        <f t="shared" ref="F45:F58" si="11">IF(C46,MIN(C45,C46)*$B$36,"")</f>
         <v/>
       </c>
       <c r="H45" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F46" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H46" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F47" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H47" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="F48" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H48" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F49" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H49" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F50" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H50" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F51" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H51" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F52" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H52" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F53" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H53" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F54" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H54" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F55" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H55" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F56" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H56" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F57" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H57" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="6:8" x14ac:dyDescent="0.45">
       <c r="F58" s="8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>